<commit_message>
add support for agents
</commit_message>
<xml_diff>
--- a/OTRSData.xlsx
+++ b/OTRSData.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="customer" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="customer_user" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="ci - Hardware" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="ci - Software" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="agent" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="53">
   <si>
     <t xml:space="preserve">customer-id</t>
   </si>
@@ -122,6 +123,66 @@
   </si>
   <si>
     <t xml:space="preserve">tomorrow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy+ao@perl-services.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two</t>
+  </si>
+  <si>
+    <t xml:space="preserve">at</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy+at@perl-services.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy+ta@perl-services.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy+aa@perl-services.de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hannah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy+hu@perl-services.de</t>
   </si>
 </sst>
 </file>
@@ -132,7 +193,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD\ HH:MM:SS"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -153,6 +214,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -197,8 +265,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -206,11 +278,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -238,36 +310,39 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>351289</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>39138</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -276,8 +351,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -295,86 +370,88 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>351289</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="1" t="n">
         <v>351289</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -383,8 +460,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -401,32 +478,35 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -435,8 +515,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Seite &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -448,50 +528,52 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.2857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.4795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -503,8 +585,192 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Seite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="dummy+ao@perl-services.de"/>
+    <hyperlink ref="D3" r:id="rId2" display="dummy+at@perl-services.de"/>
+    <hyperlink ref="D4" r:id="rId3" display="dummy+ta@perl-services.de"/>
+    <hyperlink ref="D5" r:id="rId4" display="dummy+aa@perl-services.de"/>
+    <hyperlink ref="D6" r:id="rId5" display="dummy+hm@perl-services.de"/>
+    <hyperlink ref="D7" r:id="rId6" display="dummy+hu@perl-services.de"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>